<commit_message>
Decouple “LayoutConstraintCounts” logic and optimize "moving several pages in one frame" program structure
</commit_message>
<xml_diff>
--- a/Task Schedule.xlsx
+++ b/Task Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Unity Project\DynamicScrollRect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B075593-C454-4F48-A995-4914A53ED1AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFB09220-460B-40D1-87E0-8B9D8CDD3168}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3F8D8D9B-7A01-4F6D-A5F1-2AD2EF87A740}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>任务描述</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -72,6 +72,14 @@
   </si>
   <si>
     <t>2022/3/7完成</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2022/3/8完成</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>第一层嵌套规定不能用GridLayoutGroup，解除之前的逻辑</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -145,7 +153,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -529,10 +537,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{699FD367-F921-43B0-B8F7-BBDE0CDD83E9}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.25"/>
@@ -561,29 +569,37 @@
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="46.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+    <row r="6" spans="1:2" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="43.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+    <row r="7" spans="1:2" ht="43.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+    <row r="8" spans="1:2" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="43.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+    <row r="9" spans="1:2" ht="43.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Prepare for deleting old logic codes
</commit_message>
<xml_diff>
--- a/Task Schedule.xlsx
+++ b/Task Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Unity Project\DynamicScrollRect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFB09220-460B-40D1-87E0-8B9D8CDD3168}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A0F3AE8-E972-456D-9815-6DF517F423E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3F8D8D9B-7A01-4F6D-A5F1-2AD2EF87A740}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>任务描述</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -80,6 +80,10 @@
   </si>
   <si>
     <t>第一层嵌套规定不能用GridLayoutGroup，解除之前的逻辑</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2022/3/9完成</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -540,7 +544,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.25"/>
@@ -577,6 +581,9 @@
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="B4" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="5" spans="1:2" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">

</xml_diff>

<commit_message>
Add horizontal scroll view adaptation
</commit_message>
<xml_diff>
--- a/Task Schedule.xlsx
+++ b/Task Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Unity Project\DynamicScrollRect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A0F3AE8-E972-456D-9815-6DF517F423E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A5BB669-E224-44AB-A6D8-DDD452D7EAF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3F8D8D9B-7A01-4F6D-A5F1-2AD2EF87A740}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>任务描述</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -84,6 +84,10 @@
   </si>
   <si>
     <t>2022/3/9完成</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>暂时搁置</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -544,7 +548,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.25"/>
@@ -589,6 +593,9 @@
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="B5" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="6" spans="1:2" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">

</xml_diff>

<commit_message>
Optimize "move several pages in one frame" logic
</commit_message>
<xml_diff>
--- a/Task Schedule.xlsx
+++ b/Task Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Unity Project\DynamicScrollRect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{979576B6-4427-4382-97B3-C37E9B745C7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{646F3503-E26F-436D-8B2E-2CF9151E3F74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3F8D8D9B-7A01-4F6D-A5F1-2AD2EF87A740}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>任务描述</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -276,7 +276,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="CCE8CF"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -567,8 +567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{699FD367-F921-43B0-B8F7-BBDE0CDD83E9}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.25"/>
@@ -642,6 +642,9 @@
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="B9" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="10" spans="1:2" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">

</xml_diff>

<commit_message>
Add "dynamic REMOVE specific item" logic
</commit_message>
<xml_diff>
--- a/Task Schedule.xlsx
+++ b/Task Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Unity Project\DynamicScrollRect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9CDF27A-94CD-4804-9514-A9AC6102A605}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A49F207-F21D-48EB-AC20-E7EBAD847CE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3F8D8D9B-7A01-4F6D-A5F1-2AD2EF87A740}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
   <si>
     <t>任务描述</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -112,6 +112,30 @@
   </si>
   <si>
     <t>2022/3/20完成</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2022/3/21完成</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>增加运行时动态删除指定Item逻辑</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2022/3/24完成</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>增加运行时动态删除指定SubItem逻辑</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>增加运行时动态增加Item逻辑</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>增加运行时动态增加定SubItem逻辑</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -569,10 +593,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{699FD367-F921-43B0-B8F7-BBDE0CDD83E9}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.25"/>
@@ -657,14 +681,43 @@
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="B10" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="11" spans="1:2" ht="43.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" ht="49.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="43.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="43.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="43.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="43.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="49.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add external callback function for dynamic remove logic
</commit_message>
<xml_diff>
--- a/Task Schedule.xlsx
+++ b/Task Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Unity Project\DynamicScrollRect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A49F207-F21D-48EB-AC20-E7EBAD847CE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCE73AE1-AA3A-4A38-8498-B4600B6393B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3F8D8D9B-7A01-4F6D-A5F1-2AD2EF87A740}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
   <si>
     <t>任务描述</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -136,6 +136,10 @@
   </si>
   <si>
     <t>增加运行时动态增加定SubItem逻辑</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2022/3/26完成</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -596,7 +600,7 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.25"/>
@@ -705,6 +709,9 @@
       <c r="A13" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="B13" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="14" spans="1:2" ht="43.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">

</xml_diff>

<commit_message>
Add “scroll to specific item” logic
</commit_message>
<xml_diff>
--- a/Task Schedule.xlsx
+++ b/Task Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Unity Project\DynamicScrollRect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCE73AE1-AA3A-4A38-8498-B4600B6393B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{417A6C8A-CD68-4908-B893-1B4DE871064A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3F8D8D9B-7A01-4F6D-A5F1-2AD2EF87A740}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
   <si>
     <t>任务描述</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -140,6 +140,22 @@
   </si>
   <si>
     <t>2022/3/26完成</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>增加跳转到指定subItem逻辑</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>增加跳转到指定item逻辑</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2022/3/28完成</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2022/3/27完成</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -597,10 +613,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{699FD367-F921-43B0-B8F7-BBDE0CDD83E9}">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.25"/>
@@ -717,14 +733,33 @@
       <c r="A14" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="B14" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="15" spans="1:2" ht="43.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" ht="49.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="43.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="43.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="49.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add “scroll to specific sub item” logic
</commit_message>
<xml_diff>
--- a/Task Schedule.xlsx
+++ b/Task Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Unity Project\DynamicScrollRect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{417A6C8A-CD68-4908-B893-1B4DE871064A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44620B89-1C61-488C-9504-70C093BA7EC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3F8D8D9B-7A01-4F6D-A5F1-2AD2EF87A740}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
   <si>
     <t>任务描述</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -156,6 +156,10 @@
   </si>
   <si>
     <t>2022/3/27完成</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2022/3/29完成</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -616,7 +620,7 @@
   <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.25"/>
@@ -753,12 +757,15 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="43.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" ht="43.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" ht="49.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="49.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>

</xml_diff>